<commit_message>
Data actualizada + Directorios reestructurados + Leves errores corregidos + Optimizacion de performance e implementacion de monitor de recursos dinamico en titulo de ventana
</commit_message>
<xml_diff>
--- a/REVs/REV-10-04-2025.xlsx
+++ b/REVs/REV-10-04-2025.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -601,7 +601,6 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
@@ -649,7 +648,6 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
@@ -697,7 +695,6 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
@@ -745,7 +742,6 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
@@ -793,7 +789,6 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
@@ -841,7 +836,6 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
@@ -889,7 +883,6 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
@@ -937,7 +930,6 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
@@ -985,7 +977,6 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
@@ -1033,7 +1024,6 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
@@ -1081,7 +1071,6 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr"/>
       <c r="J13" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
@@ -1129,7 +1118,6 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
@@ -1177,12 +1165,532 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
         </is>
       </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>6XS18565</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SUAVINEX SPRAY HIGIENIZANTE DE MANOS 100ML</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ANEXOS</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>6XS18552</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>SUAVINEX LOCION 500ML + GEL 500ML PACK</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ANEXOS</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>6XS18549</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>SUAVINEX BALSAMO BABY PECTORAL AROMATICO 50ML</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ANEXOS</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>6XS18553</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>SUAVINEX DEO KIDS ROLL-ON 50ML</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>6XS18562</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SUAVINEX LIMPIADOR NASAL</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ANEXOS</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>6XS18564</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>SUAVINEX SPRAY NASAL AGUA DE MAR Y ALOE 120ML +3A</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ANEXOS</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>6XS18564</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>SUAVINEX SPRAY NASAL AGUA DE MAR Y ALOE 120ML +3A</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ANEXOS</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>6XS18563</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>SUAVINEX SPRAY NASAL HIPERTONICO 120ML +3M</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ANEXOS</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Tiene IT</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>6XS18555</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>SUAVINEX MOM BALSAMO PEZON 30ML</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ANEXOS</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>6XS18556</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>SUAVINEX MOM ACEITE ESTRIAS 100ML</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ANEXOS</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>0TF27094</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>THE POTIONS CENTELLA ASIATICA WATER ESSENCE 50ML</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>TRAT.FEMENINO</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
+      <c r="Q26" t="inlineStr"/>
+      <c r="R26" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>